<commit_message>
Just editing raw data
</commit_message>
<xml_diff>
--- a/resources/sales_data.xlsx
+++ b/resources/sales_data.xlsx
@@ -402,7 +402,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,11 +447,11 @@
         <v>20</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>1500</v>
       </c>
       <c r="E2">
         <f>C2*D2</f>
-        <v>400</v>
+        <v>30000</v>
       </c>
       <c r="F2" s="1">
         <v>42832</v>
@@ -472,16 +472,17 @@
         <v>30</v>
       </c>
       <c r="D3">
-        <v>30</v>
+        <v>2000</v>
       </c>
       <c r="E3">
-        <v>200</v>
+        <f t="shared" ref="E3:E5" si="0">C3*D3</f>
+        <v>60000</v>
       </c>
       <c r="F3" s="1">
         <v>43133</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G5" si="0">F3+30</f>
+        <f t="shared" ref="G3:G5" si="1">F3+30</f>
         <v>43163</v>
       </c>
     </row>
@@ -496,16 +497,17 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E4">
-        <v>400</v>
+        <f t="shared" si="0"/>
+        <v>1200</v>
       </c>
       <c r="F4" s="1">
         <v>43099</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43129</v>
       </c>
     </row>
@@ -520,16 +522,17 @@
         <v>40</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>400</v>
       </c>
       <c r="E5">
-        <v>500</v>
+        <f t="shared" si="0"/>
+        <v>16000</v>
       </c>
       <c r="F5" s="1">
         <v>43041</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43071</v>
       </c>
     </row>

</xml_diff>